<commit_message>
Alterações Projeto Quase finalizado
</commit_message>
<xml_diff>
--- a/crud_acai.xlsx
+++ b/crud_acai.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,71 +446,806 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Preço</t>
+          <t>Preço Unitário</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unidade</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Preço Total</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Forma de Pagamento</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Cliente</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 10</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 11</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>acai</t>
+          <t>Açaí Preparado</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>R$ 25.00</t>
-        </is>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C2" t="n">
+        <v>25</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>50</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Desconhecdio</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Açai</t>
+          <t>Charque</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>R$ 25.00</t>
-        </is>
-      </c>
+        <v>500</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>g</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>30</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>desconhecido</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Açai</t>
+          <t>Farinha</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>R$ 25.00</t>
-        </is>
-      </c>
+      <c r="C4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>desconhecido</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Combo</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>R$ 35.00</t>
-        </is>
-      </c>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>25</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Farinha</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>25</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Desconhecido </t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>25</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Total de vendas:</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>50</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="n">
+        <v>25</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>25</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>desconhecido</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Farinha</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>10</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Polpa Açaí Xingu</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="n">
+        <v>30</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>30</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Polpa Açaí Xingu</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>R$ 30,00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>R$ 60,00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Polpa Açaí Xingu</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>R$ 30,00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>R$ 60,00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>R$ 25,00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>R$ 25,00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>R$ 12,50</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>R$ 12,50</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Farinha</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>2</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>R$ 10,00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>R$ 20,00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Cartão</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Açaí Preparado</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>R$ 25,00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>litro</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>R$ 25,00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Fiado</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Farinha</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>R$ 10,00</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>R$ 10,00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Fiado</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Desconhecido</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>31/10/2024</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>